<commit_message>
implementation with expected output ok!
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sfigueroa\SEA-01\308\SBA JS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CURSOS\PerScholas\SBA JavaScript Fundamentals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2C691E-E649-4576-8EAD-AFC9809E68A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7167A3-10C0-40B4-981C-9A392FC0F7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{62FC5A6E-96CC-4897-B4EE-77AC3A5FD377}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="25580" windowHeight="15260" activeTab="1" xr2:uid="{62FC5A6E-96CC-4897-B4EE-77AC3A5FD377}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>"id": number,</t>
   </si>
@@ -201,10 +201,40 @@
     <t>Calculate average</t>
   </si>
   <si>
-    <t>student ID total max points / total score</t>
-  </si>
-  <si>
     <t>AssignmentGroup.assignments</t>
+  </si>
+  <si>
+    <t>Array with Submission ID : Max Points</t>
+  </si>
+  <si>
+    <t>Array with results (learners obj)</t>
+  </si>
+  <si>
+    <t>Variable to store sum of score</t>
+  </si>
+  <si>
+    <t>Variable to store sum of Max points</t>
+  </si>
+  <si>
+    <t>sum of score</t>
+  </si>
+  <si>
+    <t>take each student from the array Results and on each submissionID</t>
+  </si>
+  <si>
+    <t>sum max points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable to store avg result </t>
+  </si>
+  <si>
+    <t>get avg and store in avg result</t>
+  </si>
+  <si>
+    <t>Update leaner object with "avg ", avg result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(created when fetching the submission info and stored in an array to be rehused) </t>
   </si>
 </sst>
 </file>
@@ -369,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -416,14 +446,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,13 +487,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>295275</xdr:colOff>
+          <xdr:colOff>298450</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>165100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>523875</xdr:colOff>
+          <xdr:colOff>527050</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -521,7 +544,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -552,11 +575,11 @@
           <xdr:col>10</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>165100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>523875</xdr:colOff>
+          <xdr:colOff>527050</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -607,7 +630,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -636,7 +659,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>314325</xdr:colOff>
+          <xdr:colOff>317500</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
@@ -693,7 +716,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -728,7 +751,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>523875</xdr:colOff>
+          <xdr:colOff>527050</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -779,7 +802,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1123,24 +1146,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F140A0-AEF2-4E71-8017-A955BDE54E34}">
-  <dimension ref="B4:H39"/>
+  <dimension ref="B4:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:G29"/>
+    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:5">
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:5" ht="15" thickBot="1"/>
     <row r="6" spans="2:5">
       <c r="C6" s="19" t="s">
         <v>19</v>
@@ -1174,7 +1197,7 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1193,7 +1216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1">
+    <row r="18" spans="2:5" ht="15" thickBot="1">
       <c r="C18" s="22" t="s">
         <v>17</v>
       </c>
@@ -1210,7 +1233,7 @@
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1238,7 +1261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1">
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="D27" s="12" t="s">
         <v>46</v>
       </c>
@@ -1246,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1">
+    <row r="28" spans="2:5" ht="15" thickBot="1">
       <c r="D28" s="12" t="s">
         <v>46</v>
       </c>
@@ -1254,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="15.75" thickBot="1">
+    <row r="29" spans="2:5" ht="15" thickBot="1">
       <c r="D29" s="12" t="s">
         <v>46</v>
       </c>
@@ -1285,13 +1308,61 @@
       </c>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" t="s">
+      <c r="B37" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:8">
       <c r="C39" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="C41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1304,21 +1375,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C05564-A3E6-4C04-8078-0FDCEDD1EC22}">
   <dimension ref="B2:N39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="0.7109375" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" customWidth="1"/>
-    <col min="14" max="14" width="103.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="35.26953125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="39.26953125" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" customWidth="1"/>
+    <col min="10" max="10" width="0.7265625" customWidth="1"/>
+    <col min="11" max="11" width="8.1796875" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" customWidth="1"/>
+    <col min="13" max="13" width="20.7265625" customWidth="1"/>
+    <col min="14" max="14" width="103.7265625" customWidth="1"/>
     <col min="15" max="15" width="81" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1330,7 +1401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15.75" thickBot="1">
+    <row r="3" spans="2:14" ht="15" thickBot="1">
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="2:14">
@@ -1353,7 +1424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1">
+    <row r="5" spans="2:14" ht="15" thickBot="1">
       <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
@@ -1367,7 +1438,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="2:14" ht="44.25" thickBot="1">
+    <row r="6" spans="2:14" ht="43" thickBot="1">
       <c r="L6" s="17" t="s">
         <v>23</v>
       </c>
@@ -1457,7 +1528,7 @@
       <c r="B14" s="13"/>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1">
+    <row r="15" spans="2:14" ht="15" thickBot="1">
       <c r="B15" s="12" t="s">
         <v>17</v>
       </c>
@@ -1480,8 +1551,8 @@
       </c>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="28" t="s">
-        <v>55</v>
+      <c r="B17" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>0</v>
@@ -1498,8 +1569,8 @@
       </c>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="28" t="s">
-        <v>55</v>
+      <c r="B19" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>1</v>
@@ -1513,8 +1584,8 @@
       </c>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="28" t="s">
-        <v>55</v>
+      <c r="B21" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>9</v>
@@ -1531,8 +1602,8 @@
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="28" t="s">
-        <v>55</v>
+      <c r="B23" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>11</v>
@@ -1552,7 +1623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15.75" thickBot="1">
+    <row r="26" spans="2:12" ht="15" thickBot="1">
       <c r="L26" s="18" t="s">
         <v>40</v>
       </c>
@@ -1573,113 +1644,68 @@
     </row>
     <row r="28" spans="2:12">
       <c r="B28" s="21"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
+      <c r="C28" s="28"/>
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="13"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:12">
       <c r="B31" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="13"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="2:13">
       <c r="B33" s="13"/>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="2:13">
       <c r="B34" s="13"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
+      <c r="C34" s="10"/>
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="13"/>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
       <c r="I35" s="9"/>
     </row>
     <row r="36" spans="2:13">
       <c r="B36" s="13"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="2:13" ht="15.75" thickBot="1">
+    <row r="37" spans="2:13" ht="15" thickBot="1">
       <c r="B37" s="15"/>
       <c r="C37" s="6" t="s">
         <v>2</v>
@@ -1712,13 +1738,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>295275</xdr:colOff>
+                    <xdr:colOff>298450</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>165100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>523875</xdr:colOff>
+                    <xdr:colOff>527050</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -1736,11 +1762,11 @@
                     <xdr:col>10</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>165100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>523875</xdr:colOff>
+                    <xdr:colOff>527050</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -1756,7 +1782,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>314325</xdr:colOff>
+                    <xdr:colOff>317500</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </from>
@@ -1784,7 +1810,7 @@
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>523875</xdr:colOff>
+                    <xdr:colOff>527050</xdr:colOff>
                     <xdr:row>22</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </to>

</xml_diff>